<commit_message>
iecodebook: update run files
</commit_message>
<xml_diff>
--- a/run/output/iecodebook/auto.xlsx
+++ b/run/output/iecodebook/auto.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="616">
   <si>
     <t>name</t>
   </si>
@@ -81,6 +81,1326 @@
   </si>
   <si>
     <t>Refused</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>_template</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>(Ignore this placeholder, but do not delete it. Thanks!)</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>choices</t>
+  </si>
+  <si>
+    <t>yesno</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>name:current</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>make</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>mpg</t>
+  </si>
+  <si>
+    <t>rep78</t>
+  </si>
+  <si>
+    <t>headroom</t>
+  </si>
+  <si>
+    <t>trunk</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>turn</t>
+  </si>
+  <si>
+    <t>displacement</t>
+  </si>
+  <si>
+    <t>gear_ratio</t>
+  </si>
+  <si>
+    <t>foreign</t>
+  </si>
+  <si>
+    <t>label:current</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Make and Model</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Mileage (mpg)</t>
+  </si>
+  <si>
+    <t>Repair Record 1978</t>
+  </si>
+  <si>
+    <t>Headroom (in.)</t>
+  </si>
+  <si>
+    <t>Trunk space (cu. ft.)</t>
+  </si>
+  <si>
+    <t>Weight (lbs.)</t>
+  </si>
+  <si>
+    <t>Length (in.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Turn Circle (ft.) </t>
+  </si>
+  <si>
+    <t>Displacement (cu. in.)</t>
+  </si>
+  <si>
+    <t>Gear Ratio</t>
+  </si>
+  <si>
+    <t>Car type</t>
+  </si>
+  <si>
+    <t>type:current</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>str17</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>choices:current</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>origin</t>
+  </si>
+  <si>
+    <t>recode:current</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>list_name</t>
+  </si>
+  <si>
+    <t>origin</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>Domestic</t>
+  </si>
+  <si>
+    <t>Foreign</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>_template</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>(Ignore this placeholder, but do not delete it. Thanks!)</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>choices</t>
+  </si>
+  <si>
+    <t>yesno</t>
+  </si>
+  <si>
+    <t>list_name</t>
+  </si>
+  <si>
+    <t>yesno</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>.d</t>
+  </si>
+  <si>
+    <t>.n</t>
+  </si>
+  <si>
+    <t>.r</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Don't Know</t>
+  </si>
+  <si>
+    <t>Not Applicable</t>
+  </si>
+  <si>
+    <t>Refused</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>_template</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>(Ignore this placeholder, but do not delete it. Thanks!)</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>choices</t>
+  </si>
+  <si>
+    <t>yesno</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>name:current</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>make</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>mpg</t>
+  </si>
+  <si>
+    <t>rep78</t>
+  </si>
+  <si>
+    <t>headroom</t>
+  </si>
+  <si>
+    <t>trunk</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>turn</t>
+  </si>
+  <si>
+    <t>displacement</t>
+  </si>
+  <si>
+    <t>gear_ratio</t>
+  </si>
+  <si>
+    <t>foreign</t>
+  </si>
+  <si>
+    <t>label:current</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Make and Model</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Mileage (mpg)</t>
+  </si>
+  <si>
+    <t>Repair Record 1978</t>
+  </si>
+  <si>
+    <t>Headroom (in.)</t>
+  </si>
+  <si>
+    <t>Trunk space (cu. ft.)</t>
+  </si>
+  <si>
+    <t>Weight (lbs.)</t>
+  </si>
+  <si>
+    <t>Length (in.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Turn Circle (ft.) </t>
+  </si>
+  <si>
+    <t>Displacement (cu. in.)</t>
+  </si>
+  <si>
+    <t>Gear Ratio</t>
+  </si>
+  <si>
+    <t>Car type</t>
+  </si>
+  <si>
+    <t>type:current</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>str17</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>choices:current</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>origin</t>
+  </si>
+  <si>
+    <t>recode:current</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>list_name</t>
+  </si>
+  <si>
+    <t>origin</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>Domestic</t>
+  </si>
+  <si>
+    <t>Foreign</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>_template</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>(Ignore this placeholder, but do not delete it. Thanks!)</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>choices</t>
+  </si>
+  <si>
+    <t>yesno</t>
+  </si>
+  <si>
+    <t>list_name</t>
+  </si>
+  <si>
+    <t>yesno</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>.d</t>
+  </si>
+  <si>
+    <t>.n</t>
+  </si>
+  <si>
+    <t>.r</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Don't Know</t>
+  </si>
+  <si>
+    <t>Not Applicable</t>
+  </si>
+  <si>
+    <t>Refused</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>_template</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>(Ignore this placeholder, but do not delete it. Thanks!)</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>choices</t>
+  </si>
+  <si>
+    <t>yesno</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>name:current</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>make</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>mpg</t>
+  </si>
+  <si>
+    <t>rep78</t>
+  </si>
+  <si>
+    <t>headroom</t>
+  </si>
+  <si>
+    <t>trunk</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>turn</t>
+  </si>
+  <si>
+    <t>displacement</t>
+  </si>
+  <si>
+    <t>gear_ratio</t>
+  </si>
+  <si>
+    <t>foreign</t>
+  </si>
+  <si>
+    <t>label:current</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Make and Model</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Mileage (mpg)</t>
+  </si>
+  <si>
+    <t>Repair Record 1978</t>
+  </si>
+  <si>
+    <t>Headroom (in.)</t>
+  </si>
+  <si>
+    <t>Trunk space (cu. ft.)</t>
+  </si>
+  <si>
+    <t>Weight (lbs.)</t>
+  </si>
+  <si>
+    <t>Length (in.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Turn Circle (ft.) </t>
+  </si>
+  <si>
+    <t>Displacement (cu. in.)</t>
+  </si>
+  <si>
+    <t>Gear Ratio</t>
+  </si>
+  <si>
+    <t>Car type</t>
+  </si>
+  <si>
+    <t>type:current</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>str17</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>choices:current</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>origin</t>
+  </si>
+  <si>
+    <t>recode:current</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>list_name</t>
+  </si>
+  <si>
+    <t>origin</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>Domestic</t>
+  </si>
+  <si>
+    <t>Foreign</t>
   </si>
   <si>
     <t>name</t>
@@ -591,408 +1911,408 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>484</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>498</v>
       </c>
       <c r="C1" t="s">
-        <v>72</v>
+        <v>512</v>
       </c>
       <c r="D1" t="s">
-        <v>86</v>
+        <v>526</v>
       </c>
       <c r="E1" t="s">
-        <v>100</v>
+        <v>540</v>
       </c>
       <c r="F1" t="s">
-        <v>114</v>
+        <v>554</v>
       </c>
       <c r="G1" t="s">
-        <v>128</v>
+        <v>568</v>
       </c>
       <c r="H1" t="s">
-        <v>140</v>
+        <v>580</v>
       </c>
       <c r="I1" t="s">
-        <v>154</v>
+        <v>594</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>485</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>499</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>513</v>
       </c>
       <c r="D2" t="s">
-        <v>87</v>
+        <v>527</v>
       </c>
       <c r="E2" t="s">
-        <v>101</v>
+        <v>541</v>
       </c>
       <c r="F2" t="s">
-        <v>115</v>
+        <v>555</v>
       </c>
       <c r="G2" t="s">
-        <v>129</v>
+        <v>569</v>
       </c>
       <c r="H2" t="s">
-        <v>141</v>
+        <v>581</v>
       </c>
       <c r="I2" t="s">
-        <v>155</v>
+        <v>595</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>486</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>500</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>514</v>
       </c>
       <c r="D3" t="s">
-        <v>88</v>
+        <v>528</v>
       </c>
       <c r="E3" t="s">
-        <v>102</v>
+        <v>542</v>
       </c>
       <c r="F3" t="s">
-        <v>116</v>
+        <v>556</v>
       </c>
       <c r="G3" t="s">
-        <v>130</v>
+        <v>570</v>
       </c>
       <c r="H3" t="s">
-        <v>142</v>
+        <v>582</v>
       </c>
       <c r="I3" t="s">
-        <v>156</v>
+        <v>596</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>487</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>501</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>515</v>
       </c>
       <c r="D4" t="s">
-        <v>89</v>
+        <v>529</v>
       </c>
       <c r="E4" t="s">
-        <v>103</v>
+        <v>543</v>
       </c>
       <c r="F4" t="s">
-        <v>117</v>
+        <v>557</v>
       </c>
       <c r="G4" t="s">
-        <v>131</v>
+        <v>571</v>
       </c>
       <c r="H4" t="s">
-        <v>143</v>
+        <v>583</v>
       </c>
       <c r="I4" t="s">
-        <v>157</v>
+        <v>597</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>488</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>502</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>516</v>
       </c>
       <c r="D5" t="s">
-        <v>90</v>
+        <v>530</v>
       </c>
       <c r="E5" t="s">
-        <v>104</v>
+        <v>544</v>
       </c>
       <c r="F5" t="s">
-        <v>118</v>
+        <v>558</v>
       </c>
       <c r="G5" t="s">
-        <v>132</v>
+        <v>572</v>
       </c>
       <c r="H5" t="s">
-        <v>144</v>
+        <v>584</v>
       </c>
       <c r="I5" t="s">
-        <v>158</v>
+        <v>598</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>489</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>503</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>517</v>
       </c>
       <c r="D6" t="s">
-        <v>91</v>
+        <v>531</v>
       </c>
       <c r="E6" t="s">
-        <v>105</v>
+        <v>545</v>
       </c>
       <c r="F6" t="s">
-        <v>119</v>
+        <v>559</v>
       </c>
       <c r="G6" t="s">
-        <v>132</v>
+        <v>572</v>
       </c>
       <c r="H6" t="s">
-        <v>145</v>
+        <v>585</v>
       </c>
       <c r="I6" t="s">
-        <v>159</v>
+        <v>599</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>490</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>504</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>518</v>
       </c>
       <c r="D7" t="s">
-        <v>92</v>
+        <v>532</v>
       </c>
       <c r="E7" t="s">
-        <v>106</v>
+        <v>546</v>
       </c>
       <c r="F7" t="s">
-        <v>120</v>
+        <v>560</v>
       </c>
       <c r="G7" t="s">
-        <v>133</v>
+        <v>573</v>
       </c>
       <c r="H7" t="s">
-        <v>146</v>
+        <v>586</v>
       </c>
       <c r="I7" t="s">
-        <v>160</v>
+        <v>600</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>491</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>505</v>
       </c>
       <c r="C8" t="s">
-        <v>79</v>
+        <v>519</v>
       </c>
       <c r="D8" t="s">
-        <v>93</v>
+        <v>533</v>
       </c>
       <c r="E8" t="s">
-        <v>107</v>
+        <v>547</v>
       </c>
       <c r="F8" t="s">
-        <v>121</v>
+        <v>561</v>
       </c>
       <c r="G8" t="s">
-        <v>134</v>
+        <v>574</v>
       </c>
       <c r="H8" t="s">
-        <v>147</v>
+        <v>587</v>
       </c>
       <c r="I8" t="s">
-        <v>161</v>
+        <v>601</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>492</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>506</v>
       </c>
       <c r="C9" t="s">
-        <v>80</v>
+        <v>520</v>
       </c>
       <c r="D9" t="s">
-        <v>94</v>
+        <v>534</v>
       </c>
       <c r="E9" t="s">
-        <v>108</v>
+        <v>548</v>
       </c>
       <c r="F9" t="s">
-        <v>122</v>
+        <v>562</v>
       </c>
       <c r="G9" t="s">
-        <v>135</v>
+        <v>575</v>
       </c>
       <c r="H9" t="s">
-        <v>148</v>
+        <v>588</v>
       </c>
       <c r="I9" t="s">
-        <v>162</v>
+        <v>602</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>493</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>507</v>
       </c>
       <c r="C10" t="s">
-        <v>81</v>
+        <v>521</v>
       </c>
       <c r="D10" t="s">
-        <v>95</v>
+        <v>535</v>
       </c>
       <c r="E10" t="s">
-        <v>109</v>
+        <v>549</v>
       </c>
       <c r="F10" t="s">
-        <v>123</v>
+        <v>563</v>
       </c>
       <c r="G10" t="s">
-        <v>135</v>
+        <v>575</v>
       </c>
       <c r="H10" t="s">
-        <v>149</v>
+        <v>589</v>
       </c>
       <c r="I10" t="s">
-        <v>163</v>
+        <v>603</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>494</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>508</v>
       </c>
       <c r="C11" t="s">
-        <v>82</v>
+        <v>522</v>
       </c>
       <c r="D11" t="s">
-        <v>96</v>
+        <v>536</v>
       </c>
       <c r="E11" t="s">
-        <v>110</v>
+        <v>550</v>
       </c>
       <c r="F11" t="s">
-        <v>124</v>
+        <v>564</v>
       </c>
       <c r="G11" t="s">
-        <v>136</v>
+        <v>576</v>
       </c>
       <c r="H11" t="s">
-        <v>150</v>
+        <v>590</v>
       </c>
       <c r="I11" t="s">
-        <v>164</v>
+        <v>604</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>495</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>509</v>
       </c>
       <c r="C12" t="s">
-        <v>83</v>
+        <v>523</v>
       </c>
       <c r="D12" t="s">
-        <v>97</v>
+        <v>537</v>
       </c>
       <c r="E12" t="s">
-        <v>111</v>
+        <v>551</v>
       </c>
       <c r="F12" t="s">
-        <v>125</v>
+        <v>565</v>
       </c>
       <c r="G12" t="s">
-        <v>137</v>
+        <v>577</v>
       </c>
       <c r="H12" t="s">
-        <v>151</v>
+        <v>591</v>
       </c>
       <c r="I12" t="s">
-        <v>165</v>
+        <v>605</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>496</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>510</v>
       </c>
       <c r="C13" t="s">
-        <v>84</v>
+        <v>524</v>
       </c>
       <c r="D13" t="s">
-        <v>98</v>
+        <v>538</v>
       </c>
       <c r="E13" t="s">
-        <v>112</v>
+        <v>552</v>
       </c>
       <c r="F13" t="s">
-        <v>126</v>
+        <v>566</v>
       </c>
       <c r="G13" t="s">
-        <v>138</v>
+        <v>578</v>
       </c>
       <c r="H13" t="s">
-        <v>152</v>
+        <v>592</v>
       </c>
       <c r="I13" t="s">
-        <v>166</v>
+        <v>606</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>497</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>511</v>
       </c>
       <c r="C14" t="s">
-        <v>85</v>
+        <v>525</v>
       </c>
       <c r="D14" t="s">
-        <v>99</v>
+        <v>539</v>
       </c>
       <c r="E14" t="s">
-        <v>113</v>
+        <v>553</v>
       </c>
       <c r="F14" t="s">
-        <v>127</v>
+        <v>567</v>
       </c>
       <c r="G14" t="s">
-        <v>139</v>
+        <v>579</v>
       </c>
       <c r="H14" t="s">
-        <v>153</v>
+        <v>593</v>
       </c>
       <c r="I14" t="s">
-        <v>167</v>
+        <v>607</v>
       </c>
     </row>
   </sheetData>
@@ -1006,68 +2326,68 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>470</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>472</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>478</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>471</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>473</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>479</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>471</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>474</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>480</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>471</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>475</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>481</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>471</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>476</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>482</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>471</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>477</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>483</v>
       </c>
     </row>
   </sheetData>
@@ -1081,35 +2401,35 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>168</v>
+        <v>608</v>
       </c>
       <c r="B1" t="s">
-        <v>170</v>
+        <v>610</v>
       </c>
       <c r="C1" t="s">
-        <v>173</v>
+        <v>613</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>609</v>
       </c>
       <c r="B2" t="s">
-        <v>171</v>
+        <v>611</v>
       </c>
       <c r="C2" t="s">
-        <v>174</v>
+        <v>614</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>169</v>
+        <v>609</v>
       </c>
       <c r="B3" t="s">
-        <v>172</v>
+        <v>612</v>
       </c>
       <c r="C3" t="s">
-        <v>175</v>
+        <v>615</v>
       </c>
     </row>
   </sheetData>

</xml_diff>